<commit_message>
-Fix the outputs pin headers spacing
</commit_message>
<xml_diff>
--- a/Rleased/BOM/H14R90.xlsx
+++ b/Rleased/BOM/H14R90.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HEXABITZ\Modules\Hardware\Modules Hardware Design\H14R90\Rleased\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HEXABITZ\Modules\Hardware\Modules Hardware Design\H14R9x-Hardware\Rleased\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A19E1DA7-B7B6-46A1-9912-392C7D65A6F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{814FE3BA-EF56-482E-AF22-14978BF83B18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -91,18 +91,9 @@
     <t>Vishay</t>
   </si>
   <si>
-    <t>PCB Header, Unshrouded, Thru 02 Straight Header, .101, AMPMODU Mod II Series</t>
-  </si>
-  <si>
     <t>TE Connectivity</t>
   </si>
   <si>
-    <t>87227-1</t>
-  </si>
-  <si>
-    <t>https://octopart.com/87227-1-te+connectivity-39512052?r=sp</t>
-  </si>
-  <si>
     <t>Conn Unshrouded Header HDR 3 POS 2.54mm Solder ST Top Entry Thru-Hole Carton</t>
   </si>
   <si>
@@ -329,6 +320,15 @@
   </si>
   <si>
     <t xml:space="preserve">4 x 5V PWM O/P + External Supply  (H14R90) </t>
+  </si>
+  <si>
+    <t>Headers &amp; Wire Housings Unshrouded 1 POS T/H</t>
+  </si>
+  <si>
+    <t>5-146280-1</t>
+  </si>
+  <si>
+    <t>https://octopart.com/5-146280-1-te+connectivity+%2F+amp-40259676?r=sp</t>
   </si>
 </sst>
 </file>
@@ -1074,6 +1074,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1093,9 +1096,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1516,7 +1516,7 @@
   <dimension ref="A2:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1561,11 +1561,11 @@
       <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="26">
         <v>0</v>
       </c>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
@@ -1573,31 +1573,31 @@
         <v>9</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="26">
+      <c r="D5" s="27">
         <v>45055</v>
       </c>
-      <c r="E5" s="27"/>
-      <c r="F5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="29"/>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="32" t="s">
-        <v>100</v>
+      <c r="B6" s="25" t="s">
+        <v>97</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="29"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="31"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="32"/>
       <c r="G6" s="2"/>
     </row>
     <row r="8" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
@@ -1622,19 +1622,19 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B9" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="D9" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>22</v>
-      </c>
       <c r="E9" s="22" t="s">
-        <v>24</v>
+        <v>100</v>
       </c>
       <c r="F9" s="16">
         <v>1</v>
@@ -1642,19 +1642,19 @@
     </row>
     <row r="10" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F10" s="16">
         <v>5</v>
@@ -1662,19 +1662,19 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C11" s="15">
         <v>1729018</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F11" s="16">
         <v>1</v>
@@ -1682,19 +1682,19 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F12" s="16">
         <v>1</v>
@@ -1702,19 +1702,19 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D13" s="17" t="s">
         <v>17</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F13" s="16">
         <v>1</v>
@@ -1722,19 +1722,19 @@
     </row>
     <row r="14" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D14" s="15" t="s">
         <v>20</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F14" s="16">
         <v>5</v>
@@ -1742,19 +1742,19 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F15" s="16">
         <v>4</v>
@@ -1762,19 +1762,19 @@
     </row>
     <row r="16" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D16" s="15" t="s">
         <v>15</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F16" s="16">
         <v>7</v>
@@ -1782,19 +1782,19 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D17" s="15" t="s">
         <v>16</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F17" s="16">
         <v>1</v>
@@ -1802,19 +1802,19 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E18" s="22" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F18" s="16">
         <v>1</v>
@@ -1822,10 +1822,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C19" s="15" t="s">
         <v>18</v>
@@ -1842,19 +1842,19 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D20" s="15" t="s">
         <v>16</v>
       </c>
       <c r="E20" s="23" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F20" s="16">
         <v>2</v>
@@ -1862,19 +1862,19 @@
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="D21" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="22" t="s">
         <v>35</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" s="22" t="s">
-        <v>38</v>
       </c>
       <c r="F21" s="16">
         <v>1</v>
@@ -1882,19 +1882,19 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D22" s="15" t="s">
         <v>20</v>
       </c>
       <c r="E22" s="22" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F22" s="16">
         <v>1</v>
@@ -1902,19 +1902,19 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B23" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" s="18" t="s">
         <v>60</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="E23" s="18" t="s">
-        <v>63</v>
       </c>
       <c r="F23" s="16">
         <v>4</v>
@@ -1922,19 +1922,19 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" s="22" t="s">
         <v>40</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="E24" s="22" t="s">
-        <v>43</v>
       </c>
       <c r="F24" s="16">
         <v>1</v>
@@ -1942,19 +1942,19 @@
     </row>
     <row r="25" spans="1:6" ht="22.8" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B25" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E25" s="24" t="s">
         <v>80</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="E25" s="24" t="s">
-        <v>83</v>
       </c>
       <c r="F25" s="20">
         <v>1</v>
@@ -1962,19 +1962,19 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D26" s="15" t="s">
         <v>16</v>
       </c>
       <c r="E26" s="22" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F26" s="21">
         <v>1</v>
@@ -1987,23 +1987,22 @@
     <mergeCell ref="D6:F6"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E9" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="E18" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="E19" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="E21" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="E24" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="E22" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="E26" r:id="rId7" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E13" r:id="rId8" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="E10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="E14" r:id="rId10" xr:uid="{BC208596-CFFC-4841-9008-85FEAC1F1913}"/>
-    <hyperlink ref="E16" r:id="rId11" xr:uid="{608D9BE0-DE64-484B-BD24-E5CEAA1C46E2}"/>
-    <hyperlink ref="E20" r:id="rId12" xr:uid="{8247B2C4-59B6-4E38-8F18-15A37292F9D6}"/>
-    <hyperlink ref="E25" r:id="rId13" xr:uid="{966C96E0-CF45-4825-87AC-06AB72ED7222}"/>
-    <hyperlink ref="E12" r:id="rId14" xr:uid="{3F162551-9AAC-4522-AC2E-98D734B996E5}"/>
+    <hyperlink ref="E18" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E19" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E21" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E24" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E22" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E26" r:id="rId6" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E13" r:id="rId7" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="E10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="E14" r:id="rId9" xr:uid="{BC208596-CFFC-4841-9008-85FEAC1F1913}"/>
+    <hyperlink ref="E16" r:id="rId10" xr:uid="{608D9BE0-DE64-484B-BD24-E5CEAA1C46E2}"/>
+    <hyperlink ref="E20" r:id="rId11" xr:uid="{8247B2C4-59B6-4E38-8F18-15A37292F9D6}"/>
+    <hyperlink ref="E25" r:id="rId12" xr:uid="{966C96E0-CF45-4825-87AC-06AB72ED7222}"/>
+    <hyperlink ref="E12" r:id="rId13" xr:uid="{3F162551-9AAC-4522-AC2E-98D734B996E5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId15"/>
-  <drawing r:id="rId16"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId14"/>
+  <drawing r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>